<commit_message>
Adição do módulo de precificação
</commit_message>
<xml_diff>
--- a/data/dim_produtos.xlsx
+++ b/data/dim_produtos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\estancia_dos_ventos\ambiente_virtual\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFC76BE-0B9E-48BA-B8EC-EFD108AD2880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486049F1-2A68-401C-BFF4-FAF1580C3C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1980" windowWidth="16995" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$478</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="424">
   <si>
     <t>Tipo</t>
   </si>
@@ -1298,13 +1297,19 @@
   </si>
   <si>
     <t>un</t>
+  </si>
+  <si>
+    <t>Batata Palha</t>
+  </si>
+  <si>
+    <t>Cogumelo champignon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1435,6 +1440,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1781,8 +1794,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2104,11 +2118,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C478"/>
+  <dimension ref="A1:C480"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2118,7 +2130,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -2213,7 +2225,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2224,7 +2236,7 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2279,7 +2291,7 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2290,7 +2302,7 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2323,7 +2335,7 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2543,7 +2555,7 @@
         <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -7373,6 +7385,28 @@
       </c>
       <c r="C478" t="s">
         <v>421</v>
+      </c>
+    </row>
+    <row r="479" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A479" t="s">
+        <v>2</v>
+      </c>
+      <c r="B479" t="s">
+        <v>422</v>
+      </c>
+      <c r="C479" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="480" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A480" t="s">
+        <v>2</v>
+      </c>
+      <c r="B480" t="s">
+        <v>423</v>
+      </c>
+      <c r="C480" t="s">
+        <v>419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>